<commit_message>
RF8 y RF 10
</commit_message>
<xml_diff>
--- a/docs/Relacional.xlsx
+++ b/docs/Relacional.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Downloads\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Documentos\Uniandes\Sistemas Transaccionales\2019-2\Interacion1\HotelAndes\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3C1AF9-9DD8-42FF-A869-FBD0B112BB7B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA8252D-1298-4688-881F-9CD00F1F274C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A378944A-33B9-46BE-AEA7-82B35769710C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="99">
   <si>
     <t>Hotel</t>
   </si>
@@ -325,13 +325,16 @@
   </si>
   <si>
     <t>IdTipoConsumo</t>
+  </si>
+  <si>
+    <t>cantidadAsistentes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,6 +352,22 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -484,7 +503,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -555,16 +574,31 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -885,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF144F5-6EDF-4548-9597-4806E21F63BC}">
-  <dimension ref="A1:AG29"/>
+  <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="35" zoomScaleNormal="35" workbookViewId="0">
-      <selection activeCell="V58" sqref="V58"/>
+    <sheetView tabSelected="1" topLeftCell="S7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V21" sqref="V21:X24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -919,11 +953,14 @@
     <col min="24" max="24" width="17.77734375" style="1" customWidth="1"/>
     <col min="25" max="25" width="12.21875" style="1" customWidth="1"/>
     <col min="26" max="26" width="11" style="1" customWidth="1"/>
-    <col min="27" max="27" width="15.5546875" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="11.5546875" style="1"/>
+    <col min="27" max="27" width="9.88671875" style="1" customWidth="1"/>
+    <col min="28" max="28" width="15.77734375" style="1" customWidth="1"/>
+    <col min="29" max="29" width="11.5546875" style="1"/>
+    <col min="30" max="30" width="16.109375" style="1" customWidth="1"/>
+    <col min="31" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -946,7 +983,7 @@
       </c>
       <c r="O1" s="22"/>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>18</v>
       </c>
@@ -981,7 +1018,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1016,7 +1053,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1051,7 +1088,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
         <v>5</v>
       </c>
@@ -1082,7 +1119,7 @@
       <c r="U6" s="22"/>
       <c r="V6" s="23"/>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
@@ -1139,7 +1176,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1196,7 +1233,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1253,7 +1290,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>17</v>
       </c>
@@ -1269,13 +1306,13 @@
         <v>22</v>
       </c>
       <c r="K11" s="22"/>
-      <c r="T11" s="24" t="s">
+      <c r="T11" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="U11" s="24"/>
-      <c r="V11" s="24"/>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="U11" s="25"/>
+      <c r="V11" s="25"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>18</v>
       </c>
@@ -1313,7 +1350,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>88</v>
       </c>
@@ -1351,7 +1388,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
@@ -1389,15 +1426,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27" t="s">
+    <row r="16" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
       <c r="G16" s="11"/>
       <c r="H16" s="26" t="s">
         <v>89</v>
@@ -1422,19 +1459,15 @@
       </c>
       <c r="W16" s="19"/>
       <c r="X16" s="20"/>
-      <c r="Z16" s="21" t="s">
+      <c r="Z16" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="AA16" s="22"/>
-      <c r="AB16" s="22"/>
-      <c r="AC16" s="23"/>
-      <c r="AE16" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF16" s="24"/>
-      <c r="AG16" s="24"/>
-    </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AA16" s="25"/>
+      <c r="AB16" s="25"/>
+      <c r="AC16" s="25"/>
+      <c r="AD16" s="25"/>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>18</v>
       </c>
@@ -1497,7 +1530,7 @@
       <c r="X17" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="Z17" s="8" t="s">
+      <c r="Z17" s="7" t="s">
         <v>18</v>
       </c>
       <c r="AA17" s="7" t="s">
@@ -1506,20 +1539,14 @@
       <c r="AB17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AC17" s="8" t="s">
+      <c r="AC17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AE17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="AG17" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD17" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -1593,17 +1620,11 @@
       <c r="AC18" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="AE18" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF18" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG18" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:33" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD18" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
@@ -1666,29 +1687,23 @@
       <c r="X19" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="Z19" s="5" t="s">
+      <c r="Z19" s="3" t="s">
         <v>48</v>
       </c>
       <c r="AA19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AB19" s="5" t="s">
+      <c r="AB19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AC19" s="5" t="s">
+      <c r="AC19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AE19" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF19" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG19" s="5" t="s">
+      <c r="AD19" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" s="26" t="s">
         <v>32</v>
       </c>
@@ -1717,8 +1732,13 @@
         <v>95</v>
       </c>
       <c r="T21" s="22"/>
-    </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="V21" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="W21" s="29"/>
+      <c r="X21" s="29"/>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>18</v>
       </c>
@@ -1765,8 +1785,17 @@
       <c r="T22" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="V22" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="W22" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="X22" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -1812,8 +1841,17 @@
       <c r="T23" s="9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="24" spans="1:33" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V23" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="W23" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="X23" s="31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>3</v>
       </c>
@@ -1860,20 +1898,29 @@
       <c r="T24" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="24" t="s">
+      <c r="V24" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="W24" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="X24" s="32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="25"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="27"/>
       <c r="L26" s="21" t="s">
         <v>45</v>
       </c>
@@ -1890,7 +1937,7 @@
       </c>
       <c r="V26" s="22"/>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>18</v>
       </c>
@@ -1949,7 +1996,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -2008,7 +2055,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:33" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>3</v>
       </c>
@@ -2069,18 +2116,15 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="S6:V6"/>
-    <mergeCell ref="Z16:AC16"/>
-    <mergeCell ref="AE16:AG16"/>
-    <mergeCell ref="T11:V11"/>
-    <mergeCell ref="P16:T16"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="V21:X21"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="O21:Q21"/>
+    <mergeCell ref="L26:O26"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Q26:S26"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="L21:M21"/>
@@ -2090,15 +2134,18 @@
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="J6:M6"/>
     <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="A26:J26"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="O21:Q21"/>
-    <mergeCell ref="L26:O26"/>
-    <mergeCell ref="A11:E11"/>
     <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="S6:V6"/>
+    <mergeCell ref="T11:V11"/>
+    <mergeCell ref="P16:T16"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="Z16:AD16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Pues algo de avance supongo
</commit_message>
<xml_diff>
--- a/docs/Relacional.xlsx
+++ b/docs/Relacional.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Documentos\Uniandes\Sistemas Transaccionales\2019-2\Interacion1\HotelAndes\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Documentos\Uniandes\Sistemas Transaccionales\2019-2\Iteracion2\HotelAndes\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA8252D-1298-4688-881F-9CD00F1F274C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70AA70E2-0AC8-4BC8-A136-250E90D9F6FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A378944A-33B9-46BE-AEA7-82B35769710C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{A378944A-33B9-46BE-AEA7-82B35769710C}"/>
   </bookViews>
   <sheets>
     <sheet name="Borrame al rato" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="131">
   <si>
     <t>Hotel</t>
   </si>
@@ -177,24 +177,15 @@
     <t>CuentaConsumo</t>
   </si>
   <si>
-    <t>PK, FK</t>
-  </si>
-  <si>
     <t>IdRol</t>
   </si>
   <si>
-    <t>FK</t>
-  </si>
-  <si>
     <t>ReservaServicio</t>
   </si>
   <si>
     <t>IdServicio</t>
   </si>
   <si>
-    <t>TipoDocumentoPersona</t>
-  </si>
-  <si>
     <t>DocumentoPersona</t>
   </si>
   <si>
@@ -328,13 +319,394 @@
   </si>
   <si>
     <t>cantidadAsistentes</t>
+  </si>
+  <si>
+    <t>Convencion</t>
+  </si>
+  <si>
+    <t>CantParticipantes</t>
+  </si>
+  <si>
+    <t>ServiciosRequeridos</t>
+  </si>
+  <si>
+    <t>IdConvencion</t>
+  </si>
+  <si>
+    <t>FinalReserva</t>
+  </si>
+  <si>
+    <t>ComienzoRerserva</t>
+  </si>
+  <si>
+    <t>NN, CK &lt; FinalReserva</t>
+  </si>
+  <si>
+    <t>NN, CK &gt; ComienzoReserva</t>
+  </si>
+  <si>
+    <t>ParticipantesConvencion</t>
+  </si>
+  <si>
+    <t>ReservaParticipanteConvencion</t>
+  </si>
+  <si>
+    <t>PlanConvencion</t>
+  </si>
+  <si>
+    <t>IdTipoDocumentoPersona</t>
+  </si>
+  <si>
+    <r>
+      <t>PK, FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;persona.idTipoDocumento&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PK, FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;persona.documento&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PK, FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;hotel.id&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PK, FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;habitacion.numeroHabitacion&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PK, FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;servicio.id&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PK, FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;planDeConsumo.id&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;tipoHabitacion.id&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PK, FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;tipoDocumento.id&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;rol.id&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PK, FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;dotacion.id&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;servicio.id&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;tipoServicio.id&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PK, FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;reserva.id&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PK, FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;factura.id&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;persona.idTipoDocumento&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;persona.documento&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;habitacion.numeroHabitacion&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;reserva.id&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PK, FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;utencilio.id&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PK, FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;producto.id&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PK, FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;convencion.id&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;tipoConsumo.id&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;planDeConsumo.id&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,16 +729,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
+      <sz val="6"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -503,7 +866,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -556,14 +919,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -574,31 +940,19 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -919,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF144F5-6EDF-4548-9597-4806E21F63BC}">
-  <dimension ref="A1:AD29"/>
+  <dimension ref="A1:AD39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V21" sqref="V21:X24"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,12 +1288,12 @@
     <col min="5" max="5" width="21.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="27.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="22.88671875" style="1" customWidth="1"/>
     <col min="10" max="10" width="17.88671875" style="1" customWidth="1"/>
     <col min="11" max="11" width="15.44140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="18.21875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5546875" style="1"/>
+    <col min="13" max="13" width="15.88671875" style="1" customWidth="1"/>
     <col min="14" max="14" width="15.77734375" style="1" customWidth="1"/>
     <col min="15" max="15" width="21.88671875" style="1" customWidth="1"/>
     <col min="16" max="16" width="22" style="1" customWidth="1"/>
@@ -952,8 +1306,8 @@
     <col min="23" max="23" width="19.5546875" style="1" customWidth="1"/>
     <col min="24" max="24" width="17.77734375" style="1" customWidth="1"/>
     <col min="25" max="25" width="12.21875" style="1" customWidth="1"/>
-    <col min="26" max="26" width="11" style="1" customWidth="1"/>
-    <col min="27" max="27" width="9.88671875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="13.21875" style="1" customWidth="1"/>
+    <col min="27" max="27" width="13.109375" style="1" customWidth="1"/>
     <col min="28" max="28" width="15.77734375" style="1" customWidth="1"/>
     <col min="29" max="29" width="11.5546875" style="1"/>
     <col min="30" max="30" width="16.109375" style="1" customWidth="1"/>
@@ -961,27 +1315,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="D1" s="21" t="s">
+      <c r="B1" s="25"/>
+      <c r="D1" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="H1" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="23"/>
+      <c r="K1" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="H1" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" s="22"/>
-      <c r="K1" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="L1" s="22"/>
-      <c r="N1" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="O1" s="22"/>
+      <c r="L1" s="23"/>
+      <c r="N1" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="23"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -993,8 +1347,8 @@
       <c r="D2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>9</v>
+      <c r="E2" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>18</v>
@@ -1026,31 +1380,31 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
@@ -1061,63 +1415,63 @@
         <v>4</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>48</v>
+        <v>110</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>48</v>
+        <v>110</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="H6" s="22"/>
-      <c r="J6" s="21" t="s">
+      <c r="G6" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="J6" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="23"/>
-      <c r="O6" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
-      <c r="S6" s="21" t="s">
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="24"/>
+      <c r="O6" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="S6" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="T6" s="22"/>
-      <c r="U6" s="22"/>
-      <c r="V6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="24"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
@@ -1181,7 +1535,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
@@ -1197,7 +1551,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>2</v>
@@ -1215,22 +1569,22 @@
         <v>6</v>
       </c>
       <c r="P8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q8" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="S8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1238,7 +1592,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>50</v>
+        <v>114</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>4</v>
@@ -1268,11 +1622,11 @@
       <c r="M9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>48</v>
+      <c r="O9" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="Q9" s="3" t="s">
         <v>12</v>
@@ -1280,8 +1634,8 @@
       <c r="S9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="T9" s="3" t="s">
-        <v>50</v>
+      <c r="T9" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="U9" s="3" t="s">
         <v>12</v>
@@ -1291,33 +1645,33 @@
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23"/>
-      <c r="G11" s="21" t="s">
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
+      <c r="G11" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="22"/>
-      <c r="J11" s="21" t="s">
+      <c r="H11" s="23"/>
+      <c r="J11" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="22"/>
-      <c r="T11" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="U11" s="25"/>
-      <c r="V11" s="25"/>
+      <c r="K11" s="23"/>
+      <c r="M11" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>18</v>
@@ -1340,25 +1694,25 @@
       <c r="K12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="T12" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="U12" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="V12" s="7" t="s">
+      <c r="M12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O12" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>1</v>
@@ -1378,25 +1732,25 @@
       <c r="K13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="T13" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="V13" s="6" t="s">
-        <v>62</v>
+      <c r="M13" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>50</v>
+      <c r="C14" s="15" t="s">
+        <v>116</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>4</v>
@@ -1408,7 +1762,7 @@
         <v>3</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>3</v>
@@ -1416,56 +1770,56 @@
       <c r="K14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="T14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="U14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="V14" s="3" t="s">
-        <v>48</v>
+      <c r="M14" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="I16" s="26"/>
-      <c r="K16" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="23"/>
-      <c r="P16" s="21" t="s">
+      <c r="H16" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" s="25"/>
+      <c r="K16" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="24"/>
+      <c r="P16" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="22"/>
-      <c r="T16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="24"/>
       <c r="U16" s="11"/>
-      <c r="V16" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="W16" s="19"/>
-      <c r="X16" s="20"/>
-      <c r="Z16" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA16" s="25"/>
-      <c r="AB16" s="25"/>
-      <c r="AC16" s="25"/>
-      <c r="AD16" s="25"/>
+      <c r="V16" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="W16" s="21"/>
+      <c r="X16" s="29"/>
+      <c r="Z16" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA16" s="21"/>
+      <c r="AB16" s="21"/>
+      <c r="AC16" s="21"/>
+      <c r="AD16" s="21"/>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
@@ -1528,7 +1882,7 @@
         <v>18</v>
       </c>
       <c r="X17" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Z17" s="7" t="s">
         <v>18</v>
@@ -1557,13 +1911,13 @@
         <v>7</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>2</v>
@@ -1572,10 +1926,10 @@
         <v>24</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>27</v>
@@ -1587,7 +1941,7 @@
         <v>2</v>
       </c>
       <c r="Q18" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R18" s="2" t="s">
         <v>1</v>
@@ -1600,28 +1954,28 @@
       </c>
       <c r="U18" s="10"/>
       <c r="V18" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="X18" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Z18" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AA18" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AB18" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AC18" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AD18" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:30" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
@@ -1635,13 +1989,13 @@
         <v>4</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>4</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G19" s="16"/>
       <c r="H19" s="3" t="s">
@@ -1651,10 +2005,10 @@
         <v>25</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="M19" s="5" t="s">
         <v>12</v>
@@ -1666,7 +2020,7 @@
         <v>3</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="R19" s="3" t="s">
         <v>4</v>
@@ -1678,20 +2032,20 @@
         <v>12</v>
       </c>
       <c r="U19" s="13"/>
-      <c r="V19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="W19" s="3" t="s">
-        <v>48</v>
+      <c r="V19" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="W19" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="X19" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="Z19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA19" s="3" t="s">
-        <v>48</v>
+      <c r="Z19" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA19" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="AB19" s="3" t="s">
         <v>4</v>
@@ -1704,39 +2058,39 @@
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="26"/>
-      <c r="I21" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="J21" s="23"/>
-      <c r="L21" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="M21" s="26"/>
-      <c r="O21" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="P21" s="22"/>
-      <c r="Q21" s="22"/>
-      <c r="S21" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="T21" s="22"/>
-      <c r="V21" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="W21" s="29"/>
-      <c r="X21" s="29"/>
+      <c r="G21" s="25"/>
+      <c r="I21" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J21" s="24"/>
+      <c r="L21" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M21" s="25"/>
+      <c r="O21" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="S21" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="T21" s="23"/>
+      <c r="V21" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="W21" s="28"/>
+      <c r="X21" s="28"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
@@ -1785,13 +2139,13 @@
       <c r="T22" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="V22" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="W22" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="X22" s="30" t="s">
+      <c r="V22" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="W22" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="X22" s="18" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1800,7 +2154,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>35</v>
@@ -1815,40 +2169,40 @@
         <v>33</v>
       </c>
       <c r="I23" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O23" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P23" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="J23" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O23" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="P23" s="9" t="s">
-        <v>80</v>
-      </c>
       <c r="Q23" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="S23" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="T23" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="V23" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="W23" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="X23" s="31" t="s">
-        <v>71</v>
+        <v>59</v>
+      </c>
+      <c r="V23" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="W23" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="X23" s="19" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:30" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1856,7 +2210,7 @@
         <v>3</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>50</v>
+        <v>129</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>12</v>
@@ -1871,20 +2225,20 @@
       <c r="G24" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I24" s="3" t="s">
-        <v>48</v>
+      <c r="I24" s="5" t="s">
+        <v>120</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="M24" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="O24" s="3" t="s">
-        <v>48</v>
+        <v>113</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="O24" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="P24" s="5" t="s">
         <v>4</v>
@@ -1892,60 +2246,60 @@
       <c r="Q24" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="S24" s="3" t="s">
-        <v>48</v>
+      <c r="S24" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="V24" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="W24" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="X24" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="V24" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="W24" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="X24" s="20" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:30" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="27"/>
-      <c r="L26" s="21" t="s">
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="29"/>
+      <c r="L26" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="Q26" s="21" t="s">
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="Q26" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="R26" s="22"/>
-      <c r="S26" s="22"/>
-      <c r="U26" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="V26" s="22"/>
+      <c r="R26" s="23"/>
+      <c r="S26" s="23"/>
+      <c r="U26" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="V26" s="23"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>9</v>
@@ -1957,10 +2311,10 @@
         <v>18</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I27" s="7" t="s">
         <v>28</v>
@@ -1978,7 +2332,7 @@
         <v>10</v>
       </c>
       <c r="O27" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Q27" s="7" t="s">
         <v>18</v>
@@ -2001,10 +2355,10 @@
         <v>2</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>6</v>
@@ -2043,16 +2397,16 @@
         <v>2</v>
       </c>
       <c r="R28" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="S28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="U28" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="V28" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:30" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -2060,25 +2414,25 @@
         <v>3</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>50</v>
+        <v>122</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>50</v>
+        <v>124</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>43</v>
@@ -2096,31 +2450,232 @@
         <v>15</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="Q29" s="3" t="s">
         <v>3</v>
       </c>
       <c r="R29" s="5" t="s">
-        <v>50</v>
+        <v>125</v>
       </c>
       <c r="S29" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="U29" s="3" t="s">
-        <v>48</v>
+      <c r="U29" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="V29" s="5" t="s">
-        <v>48</v>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A31" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="D31" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="J31" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="K31" s="21"/>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="E36" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="36">
+    <mergeCell ref="A1:B1"/>
     <mergeCell ref="V21:X21"/>
     <mergeCell ref="A26:J26"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="O21:Q21"/>
     <mergeCell ref="L26:O26"/>
+    <mergeCell ref="V16:X16"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="S6:V6"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="P16:T16"/>
+    <mergeCell ref="S21:T21"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="H16:I16"/>
@@ -2129,23 +2684,14 @@
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="L21:M21"/>
     <mergeCell ref="J11:K11"/>
+    <mergeCell ref="Z16:AD16"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="E36:H36"/>
+    <mergeCell ref="J31:K31"/>
     <mergeCell ref="K16:N16"/>
     <mergeCell ref="F21:G21"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="S6:V6"/>
-    <mergeCell ref="T11:V11"/>
-    <mergeCell ref="P16:T16"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="Z16:AD16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>